<commit_message>
State tracking - used to store information locally in a JSON. - used for remember what was the user's recent command after the introduction phase.
</commit_message>
<xml_diff>
--- a/intents/intent-definition.xlsx
+++ b/intents/intent-definition.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\College\Main Thesis\Code\Symptom-Checker-Chatbot\Symptom Checker 2.0\intents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\College\Main Thesis\Code\Symptom-Checker-Chatbot\intents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4D3D04-4BDE-4DC5-88C0-015699CCAE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043A000B-5902-44A8-A13C-14C3F884D3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>intent_name</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Quick</t>
   </si>
   <si>
-    <t>Prompt</t>
-  </si>
-  <si>
     <t>Hello! I'm [BOT], your personal symptom checker. How can I assist you today? I'm here to answer your questions, help you find what you're looking for, or simply have a friendly chat. Feel free to ask me anything!</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>Come again?</t>
   </si>
   <si>
-    <t>/@Yes:bot-bool/*/@Sure:bot-bool/*/@Yeah:bot-bool/*/@Ok:bot-bool/*/@Alright:bot-bool/*/@Agree:bot-bool/*/@Okay:bot-bool/*/@Yep:bot-bool/*/@Yup:bot-bool/*/@Go ahead:bot-bool/*/@Right:bot-bool/*/@All right:bot-bool/*/@By all means:bot-bool/*/@of course:bot-bool/*/@correct:bot-bool/*/@No:bot-bool/*/@Nah:bot-bool/*/@Nope:bot-bool/*/@Disagree:bot-bool/*/@By no means:bot-bool/*/@No thanks:bot-bool/*/@Absolutely not:bot-bool/*/@Not at all:bot-bool/*/@of course not:bot-bool/*/@incorrect:bot-bool/*</t>
-  </si>
-  <si>
     <t>PHASE-INTRO,START-INTRO</t>
   </si>
   <si>
@@ -155,6 +149,9 @@
   </si>
   <si>
     <t>Two, One</t>
+  </si>
+  <si>
+    <t>/@do mind:bot-bool/*/@don't mind:bot-bool/*/@Yes:bot-bool/*/@Sure:bot-bool/*/@Yeah:bot-bool/*/@Ok:bot-bool/*/@Alright:bot-bool/*/@Agree:bot-bool/*/@Okay:bot-bool/*/@Yep:bot-bool/*/@Yup:bot-bool/*/@Go ahead:bot-bool/*/@Right:bot-bool/*/@All right:bot-bool/*/@By all means:bot-bool/*/@of course:bot-bool/*/@correct:bot-bool/*/@No:bot-bool/*/@Nah:bot-bool/*/@Nope:bot-bool/*/@Disagree:bot-bool/*/@By no means:bot-bool/*/@No thanks:bot-bool/*/@Absolutely not:bot-bool/*/@Not at all:bot-bool/*/@of course not:bot-bool/*/@incorrect:bot-bool/*</t>
   </si>
 </sst>
 </file>
@@ -670,7 +667,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1030,7 +1027,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,24 +1091,27 @@
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>15</v>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
@@ -1139,7 +1139,7 @@
     </row>
     <row r="5" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
@@ -1153,50 +1153,50 @@
     </row>
     <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" t="s">
-        <v>33</v>
+      <c r="K6" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="K7" s="3" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
@@ -1205,51 +1205,54 @@
         <v>21</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G9" s="1">
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K9" t="s">
-        <v>33</v>
+      <c r="K9" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K7" r:id="rId1" display="/@Yes:bot-bool/*/@Sure:bot-bool/*/@Yeah:bot-bool/*/@Ok:bot-bool/*/@Alright:bot-bool/*/@Agree:bot-bool/*/@Okay:bot-bool/*/@Yep:bot-bool/*/@Yup:bot-bool/*/@Go ahead:bot-bool/*/@Right:bot-bool/*/@All right:bot-bool/*/@By all means:bot-bool/*/@of course:bot-bool/*/@correct:bot-bool/*/@No:bot-bool/*/@Nah:bot-bool/*/@Nope:bot-bool/*/@Disagree:bot-bool/*/@By no means:bot-bool/*/@No thanks:bot-bool/*/@Absolutely not:bot-bool/*/@Not at all:bot-bool/*/@of course not:bot-bool/*/@incorrect:bot-bool/*" xr:uid="{EC5F18B2-F5BB-47CB-B2C2-2796B6E7BC0C}"/>
+    <hyperlink ref="K2" r:id="rId1" display="/@do mind:bot-bool/*/@don't mind:bot-bool/*/@Yes:bot-bool/*/@Sure:bot-bool/*/@Yeah:bot-bool/*/@Ok:bot-bool/*/@Alright:bot-bool/*/@Agree:bot-bool/*/@Okay:bot-bool/*/@Yep:bot-bool/*/@Yup:bot-bool/*/@Go ahead:bot-bool/*/@Right:bot-bool/*/@All right:bot-bool/*/@By all means:bot-bool/*/@of course:bot-bool/*/@correct:bot-bool/*/@No:bot-bool/*/@Nah:bot-bool/*/@Nope:bot-bool/*/@Disagree:bot-bool/*/@By no means:bot-bool/*/@No thanks:bot-bool/*/@Absolutely not:bot-bool/*/@Not at all:bot-bool/*/@of course not:bot-bool/*/@incorrect:bot-bool/*" xr:uid="{FD003BC4-B9CD-46E0-8807-8A21B7337B66}"/>
+    <hyperlink ref="K6" r:id="rId2" display="/@do mind:bot-bool/*/@don't mind:bot-bool/*/@Yes:bot-bool/*/@Sure:bot-bool/*/@Yeah:bot-bool/*/@Ok:bot-bool/*/@Alright:bot-bool/*/@Agree:bot-bool/*/@Okay:bot-bool/*/@Yep:bot-bool/*/@Yup:bot-bool/*/@Go ahead:bot-bool/*/@Right:bot-bool/*/@All right:bot-bool/*/@By all means:bot-bool/*/@of course:bot-bool/*/@correct:bot-bool/*/@No:bot-bool/*/@Nah:bot-bool/*/@Nope:bot-bool/*/@Disagree:bot-bool/*/@By no means:bot-bool/*/@No thanks:bot-bool/*/@Absolutely not:bot-bool/*/@Not at all:bot-bool/*/@of course not:bot-bool/*/@incorrect:bot-bool/*" xr:uid="{F6C281C5-7C1B-426B-9DD2-0948AFFC0138}"/>
+    <hyperlink ref="K7" r:id="rId3" display="/@do mind:bot-bool/*/@don't mind:bot-bool/*/@Yes:bot-bool/*/@Sure:bot-bool/*/@Yeah:bot-bool/*/@Ok:bot-bool/*/@Alright:bot-bool/*/@Agree:bot-bool/*/@Okay:bot-bool/*/@Yep:bot-bool/*/@Yup:bot-bool/*/@Go ahead:bot-bool/*/@Right:bot-bool/*/@All right:bot-bool/*/@By all means:bot-bool/*/@of course:bot-bool/*/@correct:bot-bool/*/@No:bot-bool/*/@Nah:bot-bool/*/@Nope:bot-bool/*/@Disagree:bot-bool/*/@By no means:bot-bool/*/@No thanks:bot-bool/*/@Absolutely not:bot-bool/*/@Not at all:bot-bool/*/@of course not:bot-bool/*/@incorrect:bot-bool/*" xr:uid="{B6BA406B-BF48-467A-896B-F0ADDBF9A567}"/>
+    <hyperlink ref="K9" r:id="rId4" display="/@do mind:bot-bool/*/@don't mind:bot-bool/*/@Yes:bot-bool/*/@Sure:bot-bool/*/@Yeah:bot-bool/*/@Ok:bot-bool/*/@Alright:bot-bool/*/@Agree:bot-bool/*/@Okay:bot-bool/*/@Yep:bot-bool/*/@Yup:bot-bool/*/@Go ahead:bot-bool/*/@Right:bot-bool/*/@All right:bot-bool/*/@By all means:bot-bool/*/@of course:bot-bool/*/@correct:bot-bool/*/@No:bot-bool/*/@Nah:bot-bool/*/@Nope:bot-bool/*/@Disagree:bot-bool/*/@By no means:bot-bool/*/@No thanks:bot-bool/*/@Absolutely not:bot-bool/*/@Not at all:bot-bool/*/@of course not:bot-bool/*/@incorrect:bot-bool/*" xr:uid="{E16BA7B7-A8D6-4CD6-A1F3-89FD7CC73EE5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dialogue JSONs CheckUp Fulfillment w/ RulesEngine
</commit_message>
<xml_diff>
--- a/intents/intent-definition.xlsx
+++ b/intents/intent-definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\College\Main Thesis\Code\Symptom-Checker-Chatbot-2\intents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4552BE-5A72-4EA5-9B7B-C005391C178E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8242547-39BB-4518-8D7D-3413868967E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
   <si>
     <t>intent_name</t>
   </si>
@@ -203,6 +203,15 @@
   </si>
   <si>
     <t>My /@head:bot-body_part/ does not /@hurts:bot-body_condition/*I do not have a /@headache:bot-symptom/*I did not get a /@cold:bot-symptom/ yesterday*My /@legs:bot-body_part/ are not /@swollen:bot-body_condition/*My /@stomach:bot-body_part/ is not /@hurting:bot-body_condition/*I do not got /@swollen:bot-body_condition/ /@legs:bot-body_part/*My /@muscles:bot-body_part/ do not /@hurt:bot-body_condition/ and I do not have a /@fever:bot-symptom/*There is no /@pain:bot-body_condition/ in my /@chest:bot-body_part/*My /@mouth:bot-body_part/ is not /@aching:bot-body_condition/*I have not /@gained weight:bot-symptom/*I have not /@lost weight:bot-symptom/*I am not /@tired:bot-symptom/ all the time*I did not woke up in a /@cold sweat:bot-symptom/*I do not have both /@neck:bot-body_part/ and /@shoulder:bot-body_part/ /@pain:bot-body_condition/*I am not feeling /@feverish:bot-symptom/*I do notfeel a /@fever:bot-symptom/ coming*My /@neck:bot-body_part/ does not feel /@tight:bot-body_condition/*no /@respitory infections:bot-symptom/*I have not been experiencing a /@cold:bot-symptom/*I have not been feeling a /@fever:bot-symptom/ coming</t>
+  </si>
+  <si>
+    <t>en.user.query.disease.treatment</t>
+  </si>
+  <si>
+    <t>What are the treatments for /@copd:bot-disease/?*How do you treat /@asthma:bot-disease/?*How do I manage symptoms of /@cad:bot-disease/?*How do I deal with /@lung cancer:bot-disease/?*What are the ways to treat /@valve disease:bot-disease/?*What do people do with /@heart failure:bot-disease/?*What do people deal with /@arrhythmia:bot-disease/?*</t>
+  </si>
+  <si>
+    <t>en.user.confirm.symptom</t>
   </si>
 </sst>
 </file>
@@ -1076,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,6 +1426,46 @@
         <v>58</v>
       </c>
     </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K18" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1" display="/@do mind:bot-bool/*/@don't mind:bot-bool/*/@Yes:bot-bool/*/@Sure:bot-bool/*/@Yeah:bot-bool/*/@Ok:bot-bool/*/@Alright:bot-bool/*/@Agree:bot-bool/*/@Okay:bot-bool/*/@Yep:bot-bool/*/@Yup:bot-bool/*/@Go ahead:bot-bool/*/@Right:bot-bool/*/@All right:bot-bool/*/@By all means:bot-bool/*/@of course:bot-bool/*/@correct:bot-bool/*/@No:bot-bool/*/@Nah:bot-bool/*/@Nope:bot-bool/*/@Disagree:bot-bool/*/@By no means:bot-bool/*/@No thanks:bot-bool/*/@Absolutely not:bot-bool/*/@Not at all:bot-bool/*/@of course not:bot-bool/*/@incorrect:bot-bool/*" xr:uid="{FD003BC4-B9CD-46E0-8807-8A21B7337B66}"/>

</xml_diff>

<commit_message>
BP, Gender, Age, Gender Intents
</commit_message>
<xml_diff>
--- a/intents/intent-definition.xlsx
+++ b/intents/intent-definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\College\Main Thesis\Code\Symptom-Checker-Chatbot-2\intents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D1FCE1-E28D-4594-B12D-38B6CA8575A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026608BF-C84F-4B3F-8926-47FF7A4F2319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="80">
   <si>
     <t>intent_name</t>
   </si>
@@ -212,13 +212,61 @@
   </si>
   <si>
     <t>en.user.confirm.symptom</t>
+  </si>
+  <si>
+    <t>en.user.share.weight</t>
+  </si>
+  <si>
+    <t>en.user.share.blood_pressure</t>
+  </si>
+  <si>
+    <t>en.user.share.age</t>
+  </si>
+  <si>
+    <t>en.user.share.gender</t>
+  </si>
+  <si>
+    <t>I'm sorry how much do weigh again?</t>
+  </si>
+  <si>
+    <t>sys.unit-weight</t>
+  </si>
+  <si>
+    <t>/@88lbs:sys.unit-weight/*I have gained weight I am now /@70 kg:sys.unit-weight/*I am now /@70 kg:sys.unit-weight/*I lost weight I now weigh /@70 kg:sys.unit-weight/*I weigh /@50lbs:sys.unit-weight/*I'm /@30 kg:sys.unit-weight/*I am /@20kg:sys.unit-weight/*I am now /@20 pounds:sys.unit-weight/*I weigh /@50 poundss:sys.unit-weight/</t>
+  </si>
+  <si>
+    <t>Right now I am /@50 years:sys.age/ old*I am /@35 years old:sys.age/*/@67:sys.age/*I am /@30 years:sys.age/ old of age*I am /@50:sys.age/*I am /@22:sys.age/ years old</t>
+  </si>
+  <si>
+    <t>I'm sorry how old are you?</t>
+  </si>
+  <si>
+    <t>My gender is /@female:bot-gender/*/@male:bot-gender/*I am a /@boy:bot-gender/*My sex is /@male:bot-gender/</t>
+  </si>
+  <si>
+    <t>Come again what is your gender?</t>
+  </si>
+  <si>
+    <t>bot-gender</t>
+  </si>
+  <si>
+    <t>sys.age</t>
+  </si>
+  <si>
+    <t>sys.number,bot-blood_pressure_type</t>
+  </si>
+  <si>
+    <t>I'm sorry what is your blood pressure?</t>
+  </si>
+  <si>
+    <t>My bp is /@80:sys.number/ /@90:sys.number/*It is /@100:sys.number/ /@110:sys.number/*I checked my blood pressure its /@80:sys.number/ /@90:sys.number/*My /@systolic blood pressure:blood_pressure_type/ is /@100:sys.number/ and my /@diastolic blood pressure:blood_pressure_type/ is/@120:sys.number/*/@100:sys.number/ /@120:sys.number/*My blood pressure is /@80:sys.number/ /@90:sys.number/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,6 +408,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2B313F"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="33">
@@ -719,7 +772,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -729,6 +782,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1085,10 +1139,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,6 +1520,89 @@
         <v>42</v>
       </c>
     </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H26" s="5"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1" display="/@do mind:bot-bool/*/@don't mind:bot-bool/*/@Yes:bot-bool/*/@Sure:bot-bool/*/@Yeah:bot-bool/*/@Ok:bot-bool/*/@Alright:bot-bool/*/@Agree:bot-bool/*/@Okay:bot-bool/*/@Yep:bot-bool/*/@Yup:bot-bool/*/@Go ahead:bot-bool/*/@Right:bot-bool/*/@All right:bot-bool/*/@By all means:bot-bool/*/@of course:bot-bool/*/@correct:bot-bool/*/@No:bot-bool/*/@Nah:bot-bool/*/@Nope:bot-bool/*/@Disagree:bot-bool/*/@By no means:bot-bool/*/@No thanks:bot-bool/*/@Absolutely not:bot-bool/*/@Not at all:bot-bool/*/@of course not:bot-bool/*/@incorrect:bot-bool/*" xr:uid="{FD003BC4-B9CD-46E0-8807-8A21B7337B66}"/>

</xml_diff>

<commit_message>
Fulfillment Overhaul - moved all dialogue to a JSON file for better accessibility. - Introduction Phase Intents function were overhauled. - Removed State.JS
</commit_message>
<xml_diff>
--- a/intents/intent-definition.xlsx
+++ b/intents/intent-definition.xlsx
@@ -8,19 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\College\Main Thesis\Code\Symptom-Checker-Chatbot-2\intents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026608BF-C84F-4B3F-8926-47FF7A4F2319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8D4D51-CD8A-4DC0-83C5-F63F4EA4B453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="intent-definition" sheetId="1" r:id="rId1"/>
+    <sheet name="introduction" sheetId="2" r:id="rId2"/>
+    <sheet name="elicitation" sheetId="6" r:id="rId3"/>
+    <sheet name="impression" sheetId="8" r:id="rId4"/>
+    <sheet name="conclusion" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="90">
   <si>
     <t>intent_name</t>
   </si>
@@ -260,6 +264,36 @@
   </si>
   <si>
     <t>My bp is /@80:sys.number/ /@90:sys.number/*It is /@100:sys.number/ /@110:sys.number/*I checked my blood pressure its /@80:sys.number/ /@90:sys.number/*My /@systolic blood pressure:blood_pressure_type/ is /@100:sys.number/ and my /@diastolic blood pressure:blood_pressure_type/ is/@120:sys.number/*/@100:sys.number/ /@120:sys.number/*My blood pressure is /@80:sys.number/ /@90:sys.number/</t>
+  </si>
+  <si>
+    <t>en.user.start.checkup</t>
+  </si>
+  <si>
+    <t>en.user.start.query</t>
+  </si>
+  <si>
+    <t>en.user.start.greet</t>
+  </si>
+  <si>
+    <t>Hi,Hello,Greetings,Sup,Yo,Good morning,Good afternoon,Good evening</t>
+  </si>
+  <si>
+    <t>I want a checkup,Check up,Evaluate me,Give me a checkup,Test me</t>
+  </si>
+  <si>
+    <t>I have question,Query,Question,Can you answer my question,Answer me</t>
+  </si>
+  <si>
+    <t>en.user.confirm.intro</t>
+  </si>
+  <si>
+    <t>PHASE-INTRODUCTION,CHOOSE-LANGUAGE</t>
+  </si>
+  <si>
+    <t>PHASE-INTRODUCTION,CONFIRM-LANGUAGE</t>
+  </si>
+  <si>
+    <t>PHASE-INTRODUCTION,CONFIRM-TERMS</t>
   </si>
 </sst>
 </file>
@@ -772,7 +806,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -783,6 +817,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1141,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1610,4 +1646,375 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62573270-AE86-42C9-BABB-0C850BC9AFEB}">
+  <dimension ref="A1:K35"/>
+  <sheetViews>
+    <sheetView showFormulas="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" style="1" customWidth="1"/>
+    <col min="2" max="4" width="20.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26" style="1" customWidth="1"/>
+    <col min="6" max="12" width="20.7109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7BF95D6-E565-4862-977E-3F1AF0673358}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" style="7" customWidth="1"/>
+    <col min="2" max="12" width="20.7109375" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0573AC2-190D-4D04-8B3B-D7CCD0BAC1B7}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" style="7" customWidth="1"/>
+    <col min="2" max="12" width="20.7109375" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A842089C-08BD-409F-A5A1-669DD83A7C4B}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" style="7" customWidth="1"/>
+    <col min="2" max="12" width="20.7109375" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fulfillment Overhaul 2 (Missing Recalls & Query)
</commit_message>
<xml_diff>
--- a/intents/intent-definition.xlsx
+++ b/intents/intent-definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\College\Main Thesis\Code\Symptom-Checker-Chatbot-2\intents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29422244-50F1-40C5-9C7A-11CB8C5B2CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F392B189-97BD-4C28-9D8C-B93721D590E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="101">
   <si>
     <t>intent_name</t>
   </si>
@@ -296,22 +296,37 @@
     <t>en.user.share.experience</t>
   </si>
   <si>
-    <t>en.user.confirm.symptom.yes</t>
-  </si>
-  <si>
-    <t>en.user.confirm.symptom.no</t>
-  </si>
-  <si>
-    <t>/@Bone:bot-body_subject/ /@Pain:bot-body_condition_temp/*/@Rapid:bot-body_condition_temp/ /@Breath:bot-body_subject/*My /@Head:bot-body_subject/ is /@Hurts:bot-body_condition_temp/*My /@Legs:bot-body_subject/ are /@Swelling:bot-body_condition_temp/*My /@Neck:bot-body_subject/ feels /@Stiff:bot-body_condition_temp/*My /@Head:bot-body_subject/ has been /@Hurting:bot-body_condition_temp/*My /@Chest:bot-body_subject/ is /@Hurting:bot-body_condition_temp/*My /@Chest:bot-body_subject/ /@Hurts:bot-body_condition_temp/*I got /@Swollen:bot-body_condition_temp/ /@Legs:bot-body_subject/*I have /@Swollen:bot-body_condition_temp/ in my /Arms@:bot-body_subject/*I have /@Swollen:bot-body_condition_temp/ on my /Back@:bot-body_subject/*I feel /@Pain:bot-body_condition_temp/ in my /@Shoulders:bot-body_subjectt/*I have been experiencing /@Swelling:bot-body_condition_temp/ on my /@Belly:bot-body_subject/*I have /@Lost:bot-body_condition_temp/ /@Weight:bot-body_subject/*There is /@Pain:bot-body_condition_temp/ in my /@Chest:bot-body_subject/*There is /@Pain:bot-body_condition_temp/ on my /@Chest:bot-body_subject/</t>
-  </si>
-  <si>
-    <t>bot-body_subject,bot-body_condition_temp</t>
-  </si>
-  <si>
-    <t>/@Bone:bot-body_subject/ /@Pain:bot-body_condition_temp/*/@Rapid:bot-body_condition_temp/ /@Breath:bot-body_subject/*My /@Head:bot-body_subject/ is /@Hurts:bot-body_condition_temp/*My /@Legs:bot-body_subject/ are /@Swelling:bot-body_condition_temp/*My /@Neck:bot-body_subject/ feels /@Stiff:bot-body_condition_temp/*My /@Head:bot-body_subject/ has been /@Hurting:bot-body_condition_temp/*My /@Chest:bot-body_subject/ is /@Hurting:bot-body_condition_temp/*My /@Chest:bot-body_subject/ /@Hurts:bot-body_condition_temp/*My /@Hands:bot-body_subject/ is color /@Blue:bot-body_condition_temp/*I got /@Swollen:bot-body_condition_temp/ /@Legs:bot-body_subject/*I have /@Swollen:bot-body_condition_temp/ in my /Arms@:bot-body_subject/*I have /@Swollen:bot-body_condition_temp/ on my /Back@:bot-body_subject/*I feel /@Pain:bot-body_condition_temp/ in my /@Shoulders:bot-body_subjectt/*I have been experiencing /@Swelling:bot-body_condition_temp/ on my /@Belly:bot-body_subject/*I have /@Lost:bot-body_condition_temp/ /@Weight:bot-body_subject/*There is /@Pain:bot-body_condition_temp/ in my /@Chest:bot-body_subject/*There is /@Pain:bot-body_condition_temp/ on my /@Chest:bot-body_subject/</t>
-  </si>
-  <si>
-    <t>en.user.share.symptom</t>
+    <t>en.user.share.symptom.parts.yes</t>
+  </si>
+  <si>
+    <t>en.user.share.symptom.parts.no</t>
+  </si>
+  <si>
+    <t>en.user.share.symptom.yes</t>
+  </si>
+  <si>
+    <t>en.user.share.symptom.no</t>
+  </si>
+  <si>
+    <t>/@Bone:bot-body_subject/ /@Pain:bot-body_condition/*/@Rapid:bot-body_condition/ /@Breath:bot-body_subject/*My /@Head:bot-body_subject/ is /@Hurts:bot-body_condition/*My /@Legs:bot-body_subject/ are /@Swelling:bot-body_condition/*My /@Neck:bot-body_subject/ feels /@Stiff:bot-body_condition/*My /@Head:bot-body_subject/ has been /@Hurting:bot-body_condition/*My /@Chest:bot-body_subject/ is /@Hurting:bot-body_condition/*My /@Chest:bot-body_subject/ /@Hurts:bot-body_condition/*I got /@Swollen:bot-body_condition/ /@Legs:bot-body_subject/*I have /@Swollen:bot-body_condition/ in my /Arms@:bot-body_subject/*I have /@Swollen:bot-body_condition/ on my /Back@:bot-body_subject/*I feel /@Pain:bot-body_condition/ in my /@Shoulders:bot-body_subjectt/*I have been experiencing /@Swelling:bot-body_condition/ on my /@Belly:bot-body_subject/*I have /@Lost:bot-body_condition/ /@Weight:bot-body_subject/*There is /@Pain:bot-body_condition/ in my /@Chest:bot-body_subject/*There is /@Pain:bot-body_condition/ on my /@Chest:bot-body_subject/*Felt /@Pain:bot-body_condition/ in my /@Chest:bot-body_subject/</t>
+  </si>
+  <si>
+    <t>No /@Bone:bot-body_subject/ /@Pain:bot-body_condition/*No /@Rapid:bot-body_condition/ /@Breath:bot-body_subject/*My /@Head:bot-body_subject/ is not /@Hurts:bot-body_condition/*My /@Legs:bot-body_subject/ are not /@Swelling:bot-body_condition/*My /@Neck:bot-body_subject/ does not feels /@Stiff:bot-body_condition/*My /@Head:bot-body_subject/ has not been /@Hurting:bot-body_condition/*My /@Chest:bot-body_subject/ is not /@Hurting:bot-body_condition/*My /@Chest:bot-body_subject/ does not /@Hurts:bot-body_condition/*I do not got /@Swollen:bot-body_condition/ /@Legs:bot-body_subject/*I do not have /@Swollen:bot-body_condition/ in my /Arms@:bot-body_subject/*I do not have /@Swollen:bot-body_condition/ on my /Back@:bot-body_subject/*I do not feel /@Pain:bot-body_condition/ in my /@Shoulders:bot-body_subjectt/*I have not been experiencing /@Swelling:bot-body_condition/ on my /@Belly:bot-body_subject/*I have not /@Lost:bot-body_condition/ /@Weight:bot-body_subject/*There is no /@Pain:bot-body_condition/ in my /@Chest:bot-body_subject/*There is no /@Pain:bot-body_condition/ on my /@Chest:bot-body_subject/*Have not felt /@Pain:bot-body_condition/ in my /@Chest:bot-body_subject/</t>
+  </si>
+  <si>
+    <t>/@Myalgia:bot-symptom/*I have been /@Coughing:bot-symptom/ for a while now*I have been /@Coughing:bot-symptom/ since last week*I have a /@Fever:bot-symptom/*I got a /@Cold:bot-symptom/*I have signs of a /@Cold:bot-symptom/*I feel /@Dizzy:bot-symptom/*I feel a /@Fever:bot-symptom/ coming*I /@Fainted:bot-symptom/*I feel /@Anxious:bot-symptom/*Last week I felt /@Chilly:bot-symptom/*I am /@Fatigued:bot-symptom/*I woke up with a /@Cold Sweat:bot-symptom/*I also have a /@Fever:bot-symptom/*I also been feeling /@Dizzy:bot-symptom/*Feeling /@Dizzy:bot-symptom/</t>
+  </si>
+  <si>
+    <t>I have not been /@Coughing:bot-symptom/*I do not have a /@Fever:bot-symptom/*I do not got a /@Cold:bot-symptom/*I do not have signs of a /@Cold:bot-symptom/*I do not feel /@Dizzy:bot-symptom/*I do not feel a /@Fever:bot-symptom/ coming*I have not /@Fainted:bot-symptom/*I do not feel /@Anxious:bot-symptom/*I am not /@Fatigued:bot-symptom/*No /@Myalgia:bot-symptom/*My /@Fever:bot-symptom/ is gone*I no longer have a /@Fever:bot-symptom/*I no longer feel /@Fever:bot-symptom/</t>
+  </si>
+  <si>
+    <t>bot-body_subject,bot-body_condition</t>
+  </si>
+  <si>
+    <t>body-symptom</t>
+  </si>
+  <si>
+    <t>PHASE-ELICITATION</t>
   </si>
 </sst>
 </file>
@@ -1194,7 +1209,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1241,7 +1256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1257,18 +1272,13 @@
       <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="I2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1666,7 +1676,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,10 +1870,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7BF95D6-E565-4862-977E-3F1AF0673358}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,69 +1919,107 @@
     </row>
     <row r="2" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>100</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
       <c r="I2" t="s">
         <v>39</v>
+      </c>
+      <c r="K2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>100</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
+      <c r="H3" t="s">
+        <v>98</v>
+      </c>
       <c r="I3" t="s">
         <v>39</v>
+      </c>
+      <c r="K3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" t="s">
         <v>95</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>92</v>
+      </c>
+      <c r="E5" t="s">
+        <v>100</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
+      <c r="H5" t="s">
+        <v>99</v>
+      </c>
       <c r="I5" t="s">
         <v>39</v>
+      </c>
+      <c r="K5" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>93</v>
+      </c>
+      <c r="E6" t="s">
+        <v>100</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
+      <c r="H6" t="s">
+        <v>99</v>
+      </c>
       <c r="I6" t="s">
         <v>39</v>
+      </c>
+      <c r="K6" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1982,7 +2030,7 @@
     </row>
     <row r="8" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -1991,17 +2039,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>39</v>
-      </c>
-    </row>
+    <row r="9" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2021,11 +2059,6 @@
     <row r="26" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>